<commit_message>
First draft of lecture 1
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D54E1E-A117-4A4D-A843-9655B9490FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134D0B24-A863-4749-9715-F1CBDE7B9147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,7 +574,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finished lecture 2 and homework
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B55857-0E8A-9C4D-A063-5A04A8E13A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18797D1-74D1-1E4D-BC61-48721AC2B6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -68,36 +68,18 @@
     <t>Welcome, 1.4 Relative Frequency Histograms</t>
   </si>
   <si>
-    <t>1.17-1.20, 1.21-1.23, 1.26, 1.33</t>
-  </si>
-  <si>
     <t>2.1 Measures of Center, 2.2 Measures of Variability</t>
   </si>
   <si>
     <t>Find a proof for division by n-1</t>
   </si>
   <si>
-    <t>2.2 continued, 2.3 Understanding and Interperting the Standard Deviation</t>
-  </si>
-  <si>
-    <t>2.2.1, 2.2.3, 2.2.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1.1, 2.1.2, 2.1.9-10, 2.1.13, 2.1.20 </t>
-  </si>
-  <si>
     <t>Vitaly Addition</t>
   </si>
   <si>
-    <t>2.3.26 + Excel (pg 87)</t>
-  </si>
-  <si>
     <t>Excel (pg 35)</t>
   </si>
   <si>
-    <t>4.1 Probility: Events and Sample Space</t>
-  </si>
-  <si>
     <t>4.2 Calculating Probabilities Using Simple Events</t>
   </si>
   <si>
@@ -113,9 +95,6 @@
     <t>4.3 continued</t>
   </si>
   <si>
-    <t>Factorials/comb/permuts for excel</t>
-  </si>
-  <si>
     <t>4.3.1, 4.3.2, 4.3.5-12, 4.13-4.19, 4.21, 4.22, 4.24, 4.3.28, 4.3.29</t>
   </si>
   <si>
@@ -197,9 +176,6 @@
     <t>7.6.*</t>
   </si>
   <si>
-    <t>Planned Exercises</t>
-  </si>
-  <si>
     <t>Final Exam (Date TBD)</t>
   </si>
   <si>
@@ -210,6 +186,24 @@
   </si>
   <si>
     <t>1.4.17-20, 1.4.21-22, 1.4.26, 1.4.33</t>
+  </si>
+  <si>
+    <t>2.2.1, 2.2.3, 2.2.10, 2.3.26</t>
+  </si>
+  <si>
+    <t>Excel (pg 87)</t>
+  </si>
+  <si>
+    <t>4.1 Probability: Events and Sample Space</t>
+  </si>
+  <si>
+    <t>2.2 continued, 2.3 Understanding and Interpreting the Standard Deviation</t>
+  </si>
+  <si>
+    <t>Factorials/comb/permutes for excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.1, 2.1.2, 2.1.3, 2.1.9-10, 2.1.13, 2.1.20 </t>
   </si>
 </sst>
 </file>
@@ -573,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C9A758-311E-8242-9FD2-B2A99B227D87}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -583,11 +577,11 @@
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="31.1640625" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="31.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -598,19 +592,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -621,16 +612,13 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -638,18 +626,17 @@
         <v>45169</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -657,16 +644,16 @@
         <v>45174</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -674,13 +661,13 @@
         <v>45176</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -688,13 +675,13 @@
         <v>45181</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -702,13 +689,13 @@
         <v>45183</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -716,13 +703,13 @@
         <v>45188</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -730,13 +717,13 @@
         <v>45190</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -747,7 +734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -756,9 +743,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -766,13 +752,13 @@
         <v>45202</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -780,13 +766,13 @@
         <v>45204</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="4">
         <f>B12+7</f>
@@ -794,9 +780,8 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -804,13 +789,13 @@
         <v>45211</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -818,10 +803,10 @@
         <v>45216</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -831,14 +816,14 @@
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -846,13 +831,13 @@
         <v>45223</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -860,13 +845,13 @@
         <v>45225</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -874,10 +859,10 @@
         <v>45230</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -885,13 +870,13 @@
         <v>45232</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -899,10 +884,10 @@
         <v>45237</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -912,11 +897,11 @@
       <c r="C23" t="s">
         <v>7</v>
       </c>
-      <c r="E23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -927,7 +912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -938,7 +923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -946,10 +931,10 @@
         <v>45251</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="4">
         <f>B25+7</f>
@@ -957,9 +942,8 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -967,10 +951,10 @@
         <v>45258</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
@@ -978,13 +962,13 @@
         <v>45260</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
@@ -992,13 +976,13 @@
         <v>45265</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1009,7 +993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>45272</v>
       </c>
@@ -1020,7 +1004,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added hw answers to lec 4
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A6D177-A5C9-4541-81F1-83055ACD612A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED70D5-3F3A-2243-B698-C5B3F3CD795D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
moved 5 to active and finished 6
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20469AAD-58B2-8E41-B710-FF620B224BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7321EE-7A5A-A945-B0D1-8136800A09A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -252,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -260,7 +259,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -680,7 +678,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>45181</v>
       </c>
       <c r="C6" t="s">
@@ -708,7 +706,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>45188</v>
       </c>
       <c r="C8" t="s">
@@ -733,7 +731,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>45195</v>
       </c>
       <c r="C10" t="s">
@@ -836,7 +834,7 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>45223</v>
       </c>
       <c r="C18" t="s">
@@ -864,7 +862,7 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>45230</v>
       </c>
       <c r="C20" t="s">
@@ -889,7 +887,7 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>45237</v>
       </c>
       <c r="C22" t="s">
@@ -914,7 +912,7 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>45244</v>
       </c>
       <c r="C24" t="s">
@@ -981,7 +979,7 @@
       <c r="A30">
         <v>27</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>45265</v>
       </c>
       <c r="C30" t="s">

</xml_diff>

<commit_message>
fixed date of lec 9
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B58B71-B5EB-2546-926A-72BBA46017E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6391FE99-8262-1B47-9EB4-E02140F5CD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>4.4 Rules for Calculating Probabilities</t>
   </si>
   <si>
-    <t>4.4.1-4.4.37</t>
-  </si>
-  <si>
     <t>4.5 Bayes Rule</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>4.3.1, 4.3.2, 4.3.5-12, 4.13-4.19, 4.21,  4.24, 4.3.28, 4.3.29</t>
+  </si>
+  <si>
+    <t>4.4.1, 4.4.7-4.4.10, 4.4.14, 4.4.27, 4.4.29,4.4.32, 4.4.35</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,13 +599,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -619,7 +619,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -636,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
@@ -651,13 +651,13 @@
         <v>45174</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
         <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -668,10 +668,10 @@
         <v>45176</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -685,7 +685,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -699,7 +699,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -759,10 +759,10 @@
         <v>45202</v>
       </c>
       <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -773,10 +773,10 @@
         <v>45204</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -796,10 +796,10 @@
         <v>45211</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -810,7 +810,7 @@
         <v>45216</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -824,10 +824,10 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
         <v>25</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -838,10 +838,10 @@
         <v>45223</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -852,10 +852,10 @@
         <v>45225</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -866,7 +866,7 @@
         <v>45230</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -877,10 +877,10 @@
         <v>45232</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -891,7 +891,7 @@
         <v>45237</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -905,7 +905,7 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -938,7 +938,7 @@
         <v>45251</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -958,7 +958,7 @@
         <v>45258</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -969,10 +969,10 @@
         <v>45260</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -983,10 +983,10 @@
         <v>45265</v>
       </c>
       <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
         <v>38</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1011,7 +1011,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed numbering for hw
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5822EF-C04B-1E4D-A673-22502E604522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463CA473-01F1-B747-AAE7-AB509A25FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -200,10 +200,10 @@
     <t>4.2.7-4.2.10, 4.2.27, 4.2.36</t>
   </si>
   <si>
-    <t>4.3.1, 4.3.2, 4.3.5-12, 4.13-4.19, 4.21,  4.24, 4.3.28, 4.3.29</t>
-  </si>
-  <si>
     <t>4.4.1, 4.4.7-4.4.10, 4.4.14, 4.4.27, 4.4.29,4.4.32, 4.4.35</t>
+  </si>
+  <si>
+    <t>4.3.1, 4.3.2, 4.3.5-12, 4.3.13,4.3.19, 4.21,  4.24, 4.3.28, 4.3.29</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,7 +713,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
finished homework answers for 4.5
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463CA473-01F1-B747-AAE7-AB509A25FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F589175F-4308-1C4D-8139-524B5045D986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,9 +96,6 @@
     <t>4.5 Bayes Rule</t>
   </si>
   <si>
-    <t>4.5.1-4.5.15</t>
-  </si>
-  <si>
     <t>Used to be review but have to skip because of conference on 9/28</t>
   </si>
   <si>
@@ -204,6 +202,9 @@
   </si>
   <si>
     <t>4.3.1, 4.3.2, 4.3.5-12, 4.3.13,4.3.19, 4.21,  4.24, 4.3.28, 4.3.29</t>
+  </si>
+  <si>
+    <t>4.5.1-3, 4.5.9, 4.5.15</t>
   </si>
 </sst>
 </file>
@@ -577,7 +578,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,13 +600,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -619,7 +620,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -636,7 +637,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
@@ -651,13 +652,13 @@
         <v>45174</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
         <v>45</v>
-      </c>
-      <c r="E4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -668,10 +669,10 @@
         <v>45176</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -685,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -699,7 +700,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -713,7 +714,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -738,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -762,7 +763,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -773,10 +774,10 @@
         <v>45204</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -796,10 +797,10 @@
         <v>45211</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -810,7 +811,7 @@
         <v>45216</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -824,10 +825,10 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
         <v>24</v>
-      </c>
-      <c r="F17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -838,10 +839,10 @@
         <v>45223</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -852,10 +853,10 @@
         <v>45225</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -866,7 +867,7 @@
         <v>45230</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -877,10 +878,10 @@
         <v>45232</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -891,7 +892,7 @@
         <v>45237</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -905,7 +906,7 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -938,7 +939,7 @@
         <v>45251</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -958,7 +959,7 @@
         <v>45258</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -969,10 +970,10 @@
         <v>45260</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -983,10 +984,10 @@
         <v>45265</v>
       </c>
       <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" t="s">
         <v>37</v>
-      </c>
-      <c r="D30" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1011,7 +1012,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added lecture 14 and did hw
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12081819-1D87-1A44-8575-B908651A1C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF6AB40-BB92-B840-8F19-6723F4877ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -122,9 +122,6 @@
     <t>7.3, 7.5 Central Limit Theorem and Sampling Distribution of the Sample Mean</t>
   </si>
   <si>
-    <t>6.2.*</t>
-  </si>
-  <si>
     <t>6.3.*</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>6.1.18, 6.1.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.2.46-48, 6.2.68 </t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,13 +606,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -626,7 +626,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -643,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
@@ -658,13 +658,13 @@
         <v>45174</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -675,10 +675,10 @@
         <v>45176</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -692,7 +692,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -706,7 +706,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -720,7 +720,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -769,7 +769,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -817,7 +817,7 @@
         <v>45216</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
@@ -848,7 +848,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -887,7 +887,7 @@
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -912,7 +912,7 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -945,7 +945,7 @@
         <v>45251</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -965,7 +965,7 @@
         <v>45258</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -976,10 +976,10 @@
         <v>45260</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -990,10 +990,10 @@
         <v>45265</v>
       </c>
       <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
         <v>33</v>
-      </c>
-      <c r="D30" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed typo in hw
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF6AB40-BB92-B840-8F19-6723F4877ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1373410-108D-1D4E-B13A-1B6B2752A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -257,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -267,6 +267,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +585,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,7 +895,7 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="7">
         <v>45237</v>
       </c>
       <c r="C22" t="s">

</xml_diff>

<commit_message>
added 6.3 and hw
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1373410-108D-1D4E-B13A-1B6B2752A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE29DA5F-0B67-2044-B215-116F0D3DE70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18640" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -116,15 +116,9 @@
     <t>6.3 Normal Approximation to the Binomial Probability Distribution</t>
   </si>
   <si>
-    <t>6.3 Cont.</t>
-  </si>
-  <si>
     <t>7.3, 7.5 Central Limit Theorem and Sampling Distribution of the Sample Mean</t>
   </si>
   <si>
-    <t>6.3.*</t>
-  </si>
-  <si>
     <t>Exam 2 (5.2, 6.1-4, 7.3, 7.5, 7.6)</t>
   </si>
   <si>
@@ -204,6 +198,12 @@
   </si>
   <si>
     <t xml:space="preserve">6.2.46-48, 6.2.68 </t>
+  </si>
+  <si>
+    <t>Midterm Review</t>
+  </si>
+  <si>
+    <t>6.3.13, 6.3.15, 6.3.24, 6.3.28</t>
   </si>
 </sst>
 </file>
@@ -240,7 +240,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,8 +266,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +585,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,13 +607,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -627,7 +627,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -644,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
@@ -659,13 +659,13 @@
         <v>45174</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -676,10 +676,10 @@
         <v>45176</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -707,7 +707,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -721,7 +721,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -746,7 +746,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -770,7 +770,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -784,7 +784,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -814,11 +814,11 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="7">
         <v>45216</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -832,7 +832,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
@@ -849,7 +849,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -860,10 +860,7 @@
         <v>45225</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -874,7 +871,10 @@
         <v>45230</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -885,21 +885,21 @@
         <v>45232</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>45237</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -913,7 +913,7 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -942,11 +942,11 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="7">
         <v>45251</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -966,7 +966,7 @@
         <v>45258</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -977,10 +977,10 @@
         <v>45260</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -991,10 +991,10 @@
         <v>45265</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1019,7 +1019,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added hw for section 7.3
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF80A20-48CE-294A-AA42-5B6C9F36E3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE7D4FC-C565-C54A-8DB5-161AA55FC36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67200" windowHeight="37300" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed semseter planning typo
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE7D4FC-C565-C54A-8DB5-161AA55FC36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A71EE3A-4913-1D4D-8087-9192741716FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -206,7 +206,7 @@
     <t>7.5.27</t>
   </si>
   <si>
-    <t xml:space="preserve">7.3.1, 7.3.3, 7.3.15, 7.3.18, 7.3.22, 7.3.32, </t>
+    <t>7.3.1, 7.3.3, 7.3.15, 7.3.18, 7.3.22, 7.3.32</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add preojct and lecture 20
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3378338-1668-A14B-82BB-A15A1C91F2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC03639D-F6E5-F34D-91E2-D99BB8AEFDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="42700" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -215,6 +215,9 @@
 - Section 6.3: 17, 19, 24, 28
 - Section 7.3: 23, 25, 29, 32
 - Section 7.5: 26, 27, 28, 33</t>
+  </si>
+  <si>
+    <t>8.2.30, 8.2.32, 8.3.18-20, 8.3.31, 8.3.37</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -284,13 +287,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C9A758-311E-8242-9FD2-B2A99B227D87}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,7 +943,7 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="1">
         <v>45244</v>
       </c>
       <c r="C24" t="s">
@@ -958,13 +957,13 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="7">
         <v>45246</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -998,6 +997,9 @@
       <c r="C28" t="s">
         <v>24</v>
       </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">

</xml_diff>

<commit_message>
lecture 21 and hw
</commit_message>
<xml_diff>
--- a/resources/semester-planning.xlsx
+++ b/resources/semester-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitalydruker/projects/math17300/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCEA804-5757-254B-BF92-8A1DE8C80E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8431E897-844E-954C-80C5-654CF09B51F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="25100" xr2:uid="{445FF4A9-C27A-B847-9A50-7B2F6293D338}"/>
   </bookViews>
@@ -116,15 +116,6 @@
     <t>8.4 Difference between two means, 8.5 difference between proportions</t>
   </si>
   <si>
-    <t>8.7 Choosing Sample Size, Describing Bi-variate data</t>
-  </si>
-  <si>
-    <t>8.7.*</t>
-  </si>
-  <si>
-    <t>8.4.*, 8.5.*</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -220,7 +211,16 @@
     <t>https://www.ccny.cuny.edu/registrar/fall-2023-final-exam-schedule</t>
   </si>
   <si>
-    <t>Final Exam 6 pm to 8:15 pm</t>
+    <t>8.7 Choosing Sample Size</t>
+  </si>
+  <si>
+    <t>8.4.14, 8.4.19, 8.5.13, 8.5.23</t>
+  </si>
+  <si>
+    <t>8.7.1, 8.7.9, 8.7.15</t>
+  </si>
+  <si>
+    <t>Final Exam 6 pm to 8:15 pm - in our classroom</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,13 +647,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -667,7 +667,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -684,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
@@ -699,13 +699,13 @@
         <v>45174</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -716,10 +716,10 @@
         <v>45176</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -733,7 +733,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -747,7 +747,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -761,7 +761,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -786,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -810,7 +810,7 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -858,7 +858,7 @@
         <v>45216</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -872,7 +872,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -889,7 +889,7 @@
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -900,7 +900,7 @@
         <v>45225</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -914,7 +914,7 @@
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -928,7 +928,7 @@
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -939,7 +939,7 @@
         <v>45237</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -950,10 +950,10 @@
         <v>45239</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -964,10 +964,10 @@
         <v>45244</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -981,7 +981,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -992,7 +992,7 @@
         <v>45251</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1015,7 +1015,7 @@
         <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1040,10 +1040,10 @@
         <v>45265</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1073,7 +1073,7 @@
         <v>59</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>